<commit_message>
push para que rafael pushee jaja
</commit_message>
<xml_diff>
--- a/Docs/DocumentacionRequerimientos.xlsx
+++ b/Docs/DocumentacionRequerimientos.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="73">
   <si>
     <t xml:space="preserve">Requerimiento </t>
   </si>
@@ -532,6 +532,87 @@
 4) Response: 500 internal server error "ORA-00001: restricción única (ISIS2304A361720.ZONA_PK) violada
 5)Response: 500 internal server error "ORA-02291: restricción de integridad (ISIS2304A361720.FK_IDTIPOCOMIDA) violada - clave principal no encontrada
 </t>
+  </si>
+  <si>
+    <t>http://localhost:8080/RotondAndes/rest/pedidos/producto</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/RotondAndes/rest/ingredientes/8</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/RotondAndes/rest/productos/1</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/RotondAndes/rest/restaurantes/2</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/RotondAndes/rest/pedidos/mesa</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/RotondAndes/rest/pedidos/6</t>
+  </si>
+  <si>
+    <t>[DELETE] http://localhost:8080/RotondAndes/rest/pedidos/3</t>
+  </si>
+  <si>
+    <t>1)Response: 500 internal server error ("null") 
+2)Response: 403 Forbidden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">caso: todo lo del pedido 3 no esta servido aun
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) caso: el pedido no existe (ruta finalizada en 2)
+2) caso: el pedido ya fue servido (ruta terminada en 5)
+</t>
+  </si>
+  <si>
+    <t>caso: todo lo del pedido 6 no esta servido aun
+{
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Response: 200 OK
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1)Response: 500 internal server error 
+</t>
+  </si>
+  <si>
+    <t>1) caso: el pedido no existe (ruta terminada en 10)
+{}</t>
+  </si>
+  <si>
+    <t>caso: el producto existe
+JSON:
+{
+"local" : 28,
+"producto" : 42,
+"pedido" : 6
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Response: 500 internal server error 
+2) Response:500 internal server error  "ERROR": "ORA-00001: restricción única (ISIS2304A361720.PEDIDOPRODUCTO_PK) violada
+</t>
+  </si>
+  <si>
+    <t>1) caso: alguna fk no existe
+JSON:
+{
+"local" : 16,
+"producto" : 42,
+"pedido" : 1
+}
+2) caso: Ya se registro dicho producto
+JSON:
+{
+"local" : 28,
+"producto" : 42,
+"pedido" : 3
+}</t>
   </si>
 </sst>
 </file>
@@ -933,7 +1014,7 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -942,7 +1023,7 @@
     <col min="2" max="2" width="11.21875" customWidth="1"/>
     <col min="3" max="3" width="50.6640625" customWidth="1"/>
     <col min="4" max="4" width="49.88671875" customWidth="1"/>
-    <col min="5" max="5" width="49" customWidth="1"/>
+    <col min="5" max="5" width="51.44140625" customWidth="1"/>
     <col min="6" max="6" width="45.88671875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -980,7 +1061,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="360" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="331.2" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>20</v>
       </c>
@@ -991,7 +1072,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="144" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1019,7 +1100,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="374.4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1047,7 +1128,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="288" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1170,7 +1251,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="316.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="316.8" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
         <v>20</v>
       </c>
@@ -1179,121 +1260,184 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>10</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C18" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D18" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C19" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>11</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E20" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B21" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>12</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E22" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B23" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>13</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E24" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B25" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>14</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E26" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B27" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>15</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E28" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B29" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>16</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E30" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B31" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>17</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C32" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B33" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C33" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>18</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C34" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D34" t="s">
+        <v>23</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B35" s="3" t="s">
         <v>20</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1303,11 +1447,20 @@
     <hyperlink ref="E6" r:id="rId3" xr:uid="{9210A2B4-56C4-4EAB-853C-FCBD1212C870}"/>
     <hyperlink ref="E10" r:id="rId4" xr:uid="{9203759E-70FD-44DB-9B58-255555D4E518}"/>
     <hyperlink ref="E14" r:id="rId5" xr:uid="{D9CFCC06-1785-4BF5-BB99-1B388D1C00DE}"/>
+    <hyperlink ref="E18" r:id="rId6" xr:uid="{1553C123-9C9B-4C0E-BA7B-D6EC59A37DE9}"/>
+    <hyperlink ref="E20" r:id="rId7" xr:uid="{70BF5B49-7BDE-4595-B2C4-DBA1BD16BE08}"/>
+    <hyperlink ref="E22" r:id="rId8" xr:uid="{7F00B29F-A7BA-44AD-9A5D-34CB57926046}"/>
+    <hyperlink ref="E24" r:id="rId9" xr:uid="{2919FDDB-3881-48A5-B456-B6A3CE27FB08}"/>
+    <hyperlink ref="E26" r:id="rId10" xr:uid="{DB876AD8-8DC4-44C8-B758-6CF2FCDB3154}"/>
+    <hyperlink ref="E28" r:id="rId11" xr:uid="{5C2EA967-FADE-44ED-B322-710777A39FEB}"/>
+    <hyperlink ref="E30" r:id="rId12" xr:uid="{10814791-A8C2-43AD-90E0-EE8760CF8340}"/>
+    <hyperlink ref="E32" r:id="rId13" xr:uid="{CCD15EAB-672B-485F-86D6-DFBB855574A4}"/>
+    <hyperlink ref="E34" r:id="rId14" display="http://localhost:8080/RotondAndes/rest/pedidos/3" xr:uid="{32FE6DA2-9FCE-454D-B399-5AD0A9ED2B88}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId6"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId15"/>
   <tableParts count="1">
-    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId16"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
FINAL FINAL FINAL, NO DA MAS
</commit_message>
<xml_diff>
--- a/Docs/DocumentacionRequerimientos.xlsx
+++ b/Docs/DocumentacionRequerimientos.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="89">
   <si>
     <t xml:space="preserve">Requerimiento </t>
   </si>
@@ -573,10 +573,6 @@
 }</t>
   </si>
   <si>
-    <t xml:space="preserve">Response: 200 OK
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">1)Response: 500 internal server error 
 </t>
   </si>
@@ -612,6 +608,180 @@
 "local" : 28,
 "producto" : 42,
 "pedido" : 3
+}</t>
+  </si>
+  <si>
+    <t>caso: el producto existe
+JSON:
+{
+"local" : 28,
+"producto" : 123,
+"pedido" : 6
+}</t>
+  </si>
+  <si>
+    <t>1)Response: 500 internal server error 
+2) Response:500 internal server error  "ERROR": "ORA-00001: restricción única (ISIS2304A361720.PEDIDOPRODUCTO_PK) violada</t>
+  </si>
+  <si>
+    <t>1)Response: 500 internal server error 
+2) Response: 403 Forbidden</t>
+  </si>
+  <si>
+    <t>1) Response: 500 internal server error 
+2) Response: 403 Forbidden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Response: 500 internal server error </t>
+  </si>
+  <si>
+    <t>1) Response: 500 internal server error ("ERROR": "ORA-00001: restricción única (ISIS2304A361720.PEDIDOMESA_PK) violada")
+2) Response: 500 internal server error ("ERROR": "ORA-00001: restricción única (ISIS2304A361720.PEDIDO_PK) violada")</t>
+  </si>
+  <si>
+    <t>1) caso: alguna fk no existe
+JSON:
+{
+"local" : 16,
+"producto" : 42,
+"pedido" : 1
+}
+2)caso: Ya se registro dicho producto
+JSON:
+{
+"local" : 28,
+"producto" : 42,
+"pedido" : 3
+}</t>
+  </si>
+  <si>
+    <t>caso: los dos ingredientes existen
+JSON:
+{
+ "usuarioRestaurante" : 3424,
+ "local" : 2,
+ "idIngrediente" : 2
+}</t>
+  </si>
+  <si>
+    <t>1)caso: algun ingrediente no existe
+JSON:
+{
+ "usuarioRestaurante" : 3424,
+ "local" : 2,
+ "idIngrediente" : 1
+}
+2)caso: el ingrediente es el mismo
+JSON:
+{
+ "usuarioRestaurante" : 3424,
+ "local" : 2,
+ "idIngrediente" : 8
+}</t>
+  </si>
+  <si>
+    <t>caso: los dos productos existen
+JSON:
+{
+ "usuarioRestaurante" : 3424,
+ "local" : 2,
+ "idProducto" : 42
+}</t>
+  </si>
+  <si>
+    <t>1)caso: algun ingrediente no existe
+JSON:
+{
+ "usuarioRestaurante" : 3424,
+ "local" : 2,
+ "idProducto" : 16
+}
+2) caso: el ingrediente es el mismo
+JSON:
+{
+ "usuarioRestaurante" : 3424,
+ "local" : 2,
+ "idProducto" : 1
+}</t>
+  </si>
+  <si>
+    <t>caso: los dos productos existen
+JSON:
+{
+ "usuarioRestaurante" : 3424,
+ "producto" : 876
+}</t>
+  </si>
+  <si>
+    <t>caso: no es un usuario restaurante 
+JSON:
+{
+ "usuarioRestaurante" : 24234,
+ "producto" : 876
+}</t>
+  </si>
+  <si>
+    <t>caso: los dos productos existen
+JSON:
+{
+"local" : 28,
+"producto" : 42,
+"pedido" : 1,
+"equivalencias" : [876]
+}</t>
+  </si>
+  <si>
+    <t>1)caso: alguna fk no existe
+JSON:
+{
+"local" : 16,
+"producto" : 42,
+"pedido" : 1,
+"equivalencias" : [876]
+}
+2)caso: Ya se registro dicho producto
+JSON:
+{
+"local" : 28,
+"producto" : 42,
+"pedido" : 3,
+"equivalencias" : [123]
+}</t>
+  </si>
+  <si>
+    <t>caso: los dos productos existen
+{
+ "idMesa":3,
+ "pedidos":[{ "idPedido":10,
+ "productos":[{"local":2,"idProducto":876,"equivalencias":[253]},
+ {"local":2,"idProducto":253},
+ {"local":2,"idMenu":1}]},
+ {"idPedido":11,
+ "productos":[{"local":2,"idProducto":876,"equivalencias":[253]},
+ {"local":2,"idProducto":253},
+ {"local":2,"idMenu":1}]}]
+}</t>
+  </si>
+  <si>
+    <t>1)caso: El idMesa y/o idPedido ya existe
+{
+ "idMesa":1,
+ "pedidos":[{ "idPedido": 6,
+ "productos":[{"local":2,"idProducto":876,"equivalencias":[253]},
+ {"local":2,"idProducto":253},
+ {"local":2,"idMenu":1}]},
+ {"idPedido":1,
+ "productos":[{"local":2,"idProducto":876,"equivalencias":[253]},
+ {"local":2,"idProducto":253},
+ {"local":2,"idMenu":1}]}]
+}
+2) caso: el pedido ya fue servido
+{
+ "idMesa":3,
+ "pedidos":[{ "idPedido": 5,
+ "productos":[{"local":2,"idProducto":876,"equivalencias":[253]},
+ {"local":2,"idProducto":253},
+ {"local":2,"idMenu":1}]}]
 }</t>
   </si>
 </sst>
@@ -1013,8 +1183,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA3B7241-BBE2-4DC1-8DBD-43F792D30A93}">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1268,7 +1438,7 @@
         <v>19</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D18" t="s">
         <v>23</v>
@@ -1282,106 +1452,178 @@
         <v>20</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>11</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="C20" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="E20" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="B21" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C21" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>12</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="C22" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D22" t="s">
+        <v>23</v>
+      </c>
       <c r="E22" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="244.8" x14ac:dyDescent="0.3">
       <c r="B23" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C23" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>13</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="C24" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D24" t="s">
+        <v>23</v>
+      </c>
       <c r="E24" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="B25" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C25" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>14</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="C26" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D26" t="s">
+        <v>23</v>
+      </c>
       <c r="E26" s="4" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
       <c r="B27" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C27" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>15</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="C28" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D28" t="s">
+        <v>23</v>
+      </c>
       <c r="E28" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="B29" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C29" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>16</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="C30" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D30" t="s">
+        <v>23</v>
+      </c>
       <c r="E30" s="4" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
       <c r="B31" s="3" t="s">
         <v>20</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
@@ -1395,7 +1637,7 @@
         <v>66</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>67</v>
+        <v>23</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>61</v>
@@ -1406,10 +1648,10 @@
         <v>20</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">

</xml_diff>